<commit_message>
Created new damage curves based on JRC
</commit_message>
<xml_diff>
--- a/LUISA_damage_info_curves.xlsx
+++ b/LUISA_damage_info_curves.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://deltares-my.sharepoint.com/personal/ted_buskop_deltares_nl/Documents/Documents/GitHub/FLOODS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_7BE859CF2764FA39C2903889AFA03F75A90CA07F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="111" documentId="11_7BE859CF2764FA39C2903889AFA03F75A90CA07F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4398BE8F-3ABD-4C1A-B963-A801F227E4CC}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
   <si>
     <t>Land use code</t>
   </si>
@@ -243,6 +243,18 @@
   </si>
   <si>
     <t>Sea and ocean</t>
+  </si>
+  <si>
+    <t>residential</t>
+  </si>
+  <si>
+    <t>commercial</t>
+  </si>
+  <si>
+    <t>industrial</t>
+  </si>
+  <si>
+    <t>agricultural</t>
   </si>
 </sst>
 </file>
@@ -253,7 +265,7 @@
     <numFmt numFmtId="164" formatCode="#,##0.00%"/>
     <numFmt numFmtId="165" formatCode="#,##0%"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -279,6 +291,13 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -298,7 +317,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -328,11 +347,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFC6C6C6"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -376,8 +405,15 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -681,11 +717,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:X47"/>
+  <dimension ref="A1:AA47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M2" sqref="M2"/>
+      <selection pane="bottomLeft" activeCell="W42" sqref="W42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -714,9 +750,10 @@
     <col min="22" max="22" width="23.28515625" style="14" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="18.28515625" style="14" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="13.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -786,8 +823,20 @@
       <c r="W1" s="7" t="s">
         <v>22</v>
       </c>
+      <c r="X1" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y1" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z1" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA1" s="15" t="s">
+        <v>72</v>
+      </c>
     </row>
-    <row r="2" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1111</v>
       </c>
@@ -863,9 +912,20 @@
       <c r="W2" s="9">
         <v>0.05</v>
       </c>
-      <c r="X2" s="10"/>
+      <c r="X2" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="Y2" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="Z2" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA2" s="9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1121</v>
       </c>
@@ -941,9 +1001,20 @@
       <c r="W3" s="9">
         <v>0</v>
       </c>
-      <c r="X3" s="10"/>
+      <c r="X3" s="10">
+        <v>0.6</v>
+      </c>
+      <c r="Y3" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="Z3" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1122</v>
       </c>
@@ -1019,9 +1090,20 @@
       <c r="W4" s="9">
         <v>0</v>
       </c>
-      <c r="X4" s="10"/>
+      <c r="X4" s="10">
+        <v>0.6</v>
+      </c>
+      <c r="Y4" s="9">
+        <v>0.3</v>
+      </c>
+      <c r="Z4" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="AA4" s="9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1123</v>
       </c>
@@ -1097,9 +1179,20 @@
       <c r="W5" s="9">
         <v>0</v>
       </c>
-      <c r="X5" s="10"/>
+      <c r="X5" s="10">
+        <v>0.6</v>
+      </c>
+      <c r="Y5" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="AA5" s="9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>1130</v>
       </c>
@@ -1175,9 +1268,20 @@
       <c r="W6" s="9">
         <v>0</v>
       </c>
-      <c r="X6" s="10"/>
+      <c r="X6" s="10">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>1210</v>
       </c>
@@ -1218,22 +1322,22 @@
         <v>236.1336409725966</v>
       </c>
       <c r="M7" s="3">
-        <v>0.7</v>
+        <v>0.45</v>
       </c>
       <c r="N7" s="3">
         <f t="shared" si="3"/>
-        <v>330.58709736163519</v>
+        <v>212.52027687533695</v>
       </c>
       <c r="O7" s="3">
         <f t="shared" si="4"/>
-        <v>165.29354868081759</v>
+        <v>106.26013843766847</v>
       </c>
       <c r="P7" s="3">
         <v>0</v>
       </c>
       <c r="Q7" s="3">
         <f t="shared" si="5"/>
-        <v>495.88064604245278</v>
+        <v>318.78041531300539</v>
       </c>
       <c r="R7" s="9">
         <v>0.05</v>
@@ -1253,9 +1357,20 @@
       <c r="W7" s="9">
         <v>0</v>
       </c>
-      <c r="X7" s="10"/>
+      <c r="X7" s="10">
+        <v>1</v>
+      </c>
+      <c r="Y7" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="Z7" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="AA7" s="9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>1221</v>
       </c>
@@ -1289,29 +1404,29 @@
         <v>472.26728194519319</v>
       </c>
       <c r="K8" s="3">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="L8" s="3">
         <f t="shared" si="2"/>
-        <v>236.1336409725966</v>
+        <v>0</v>
       </c>
       <c r="M8" s="3">
-        <v>0.7</v>
+        <v>0.05</v>
       </c>
       <c r="N8" s="3">
         <f t="shared" si="3"/>
-        <v>330.58709736163519</v>
+        <v>23.613364097259662</v>
       </c>
       <c r="O8" s="3">
         <f t="shared" si="4"/>
-        <v>165.29354868081759</v>
+        <v>0</v>
       </c>
       <c r="P8" s="3">
         <v>0</v>
       </c>
       <c r="Q8" s="3">
         <f t="shared" si="5"/>
-        <v>495.88064604245278</v>
+        <v>23.613364097259662</v>
       </c>
       <c r="R8" s="9">
         <v>0.1</v>
@@ -1331,9 +1446,20 @@
       <c r="W8" s="9">
         <v>0.1</v>
       </c>
-      <c r="X8" s="10"/>
+      <c r="X8" s="10">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="9">
+        <v>1</v>
+      </c>
+      <c r="AA8" s="9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>1222</v>
       </c>
@@ -1409,9 +1535,20 @@
       <c r="W9" s="9">
         <v>0.6</v>
       </c>
-      <c r="X9" s="10"/>
+      <c r="X9" s="10">
+        <v>1</v>
+      </c>
+      <c r="Y9" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="9">
+        <v>1</v>
+      </c>
+      <c r="AA9" s="9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>1230</v>
       </c>
@@ -1452,22 +1589,22 @@
         <v>236.1336409725966</v>
       </c>
       <c r="M10" s="3">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="N10" s="3">
         <f t="shared" si="3"/>
-        <v>330.58709736163519</v>
+        <v>141.68018458355795</v>
       </c>
       <c r="O10" s="3">
         <f t="shared" si="4"/>
-        <v>165.29354868081759</v>
+        <v>70.840092291778973</v>
       </c>
       <c r="P10" s="3">
         <v>0</v>
       </c>
       <c r="Q10" s="3">
         <f t="shared" si="5"/>
-        <v>495.88064604245278</v>
+        <v>212.52027687533692</v>
       </c>
       <c r="R10" s="9">
         <v>0.1</v>
@@ -1487,9 +1624,20 @@
       <c r="W10" s="9">
         <v>0.2</v>
       </c>
-      <c r="X10" s="10"/>
+      <c r="X10" s="10">
+        <v>1</v>
+      </c>
+      <c r="Y10" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z10" s="9">
+        <v>1</v>
+      </c>
+      <c r="AA10" s="9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>1241</v>
       </c>
@@ -1565,9 +1713,20 @@
       <c r="W11" s="9">
         <v>0.6</v>
       </c>
-      <c r="X11" s="10"/>
+      <c r="X11" s="10">
+        <v>1</v>
+      </c>
+      <c r="Y11" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z11" s="9">
+        <v>1</v>
+      </c>
+      <c r="AA11" s="9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>1242</v>
       </c>
@@ -1643,9 +1802,20 @@
       <c r="W12" s="9">
         <v>0.6</v>
       </c>
-      <c r="X12" s="10"/>
+      <c r="X12" s="10">
+        <v>1</v>
+      </c>
+      <c r="Y12" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z12" s="9">
+        <v>1</v>
+      </c>
+      <c r="AA12" s="9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>1310</v>
       </c>
@@ -1686,22 +1856,22 @@
         <v>236.1336409725966</v>
       </c>
       <c r="M13" s="3">
-        <v>7.0000000000000007E-2</v>
+        <v>0.01</v>
       </c>
       <c r="N13" s="3">
         <f t="shared" si="3"/>
-        <v>33.058709736163529</v>
+        <v>4.7226728194519323</v>
       </c>
       <c r="O13" s="3">
         <f t="shared" si="4"/>
-        <v>16.529354868081764</v>
+        <v>2.3613364097259661</v>
       </c>
       <c r="P13" s="3">
         <v>0</v>
       </c>
       <c r="Q13" s="3">
         <f t="shared" si="5"/>
-        <v>49.58806460424529</v>
+        <v>7.084009229177898</v>
       </c>
       <c r="R13" s="9">
         <v>0.2</v>
@@ -1721,9 +1891,20 @@
       <c r="W13" s="9">
         <v>0</v>
       </c>
-      <c r="X13" s="10"/>
+      <c r="X13" s="10">
+        <v>1</v>
+      </c>
+      <c r="Y13" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z13" s="9">
+        <v>1</v>
+      </c>
+      <c r="AA13" s="9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>1320</v>
       </c>
@@ -1764,22 +1945,22 @@
         <v>236.1336409725966</v>
       </c>
       <c r="M14" s="3">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="N14" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>4.7226728194519323</v>
       </c>
       <c r="O14" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>2.3613364097259661</v>
       </c>
       <c r="P14" s="3">
         <v>0</v>
       </c>
       <c r="Q14" s="3">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>7.084009229177898</v>
       </c>
       <c r="R14" s="9">
         <v>0</v>
@@ -1799,9 +1980,20 @@
       <c r="W14" s="9">
         <v>0</v>
       </c>
-      <c r="X14" s="10"/>
+      <c r="X14" s="10">
+        <v>1</v>
+      </c>
+      <c r="Y14" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z14" s="9">
+        <v>1</v>
+      </c>
+      <c r="AA14" s="9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="15" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>1330</v>
       </c>
@@ -1835,29 +2027,29 @@
         <v>472.26728194519319</v>
       </c>
       <c r="K15" s="3">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="L15" s="3">
         <f t="shared" si="2"/>
-        <v>236.1336409725966</v>
+        <v>141.68018458355795</v>
       </c>
       <c r="M15" s="3">
-        <v>0.7</v>
+        <v>0.4</v>
       </c>
       <c r="N15" s="3">
         <f t="shared" si="3"/>
-        <v>330.58709736163519</v>
+        <v>188.9069127780773</v>
       </c>
       <c r="O15" s="3">
         <f t="shared" si="4"/>
-        <v>165.29354868081759</v>
+        <v>56.672073833423184</v>
       </c>
       <c r="P15" s="3">
         <v>0</v>
       </c>
       <c r="Q15" s="3">
         <f t="shared" si="5"/>
-        <v>495.88064604245278</v>
+        <v>245.57898661150048</v>
       </c>
       <c r="R15" s="9">
         <v>0.3</v>
@@ -1877,9 +2069,20 @@
       <c r="W15" s="9">
         <v>0</v>
       </c>
-      <c r="X15" s="10"/>
+      <c r="X15" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="Y15" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z15" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="AA15" s="9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>1410</v>
       </c>
@@ -1920,22 +2123,22 @@
         <v>236.1336409725966</v>
       </c>
       <c r="M16" s="3">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="N16" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>47.226728194519325</v>
       </c>
       <c r="O16" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>23.613364097259662</v>
       </c>
       <c r="P16" s="3">
         <v>0</v>
       </c>
       <c r="Q16" s="3">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>70.840092291778987</v>
       </c>
       <c r="R16" s="9">
         <v>0</v>
@@ -1955,9 +2158,20 @@
       <c r="W16" s="9">
         <v>0</v>
       </c>
-      <c r="X16" s="10"/>
+      <c r="X16" s="10">
+        <v>1</v>
+      </c>
+      <c r="Y16" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z16" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA16" s="9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>1421</v>
       </c>
@@ -2033,9 +2247,20 @@
       <c r="W17" s="9">
         <v>0</v>
       </c>
-      <c r="X17" s="10"/>
+      <c r="X17" s="10">
+        <v>1</v>
+      </c>
+      <c r="Y17" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z17" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA17" s="9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="18" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>1422</v>
       </c>
@@ -2111,9 +2336,20 @@
       <c r="W18" s="9">
         <v>0</v>
       </c>
-      <c r="X18" s="10"/>
+      <c r="X18" s="10">
+        <v>1</v>
+      </c>
+      <c r="Y18" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z18" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA18" s="9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="19" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>2110</v>
       </c>
@@ -2190,9 +2426,20 @@
       <c r="W19" s="9">
         <v>0</v>
       </c>
-      <c r="X19" s="10"/>
+      <c r="X19" s="10">
+        <v>1</v>
+      </c>
+      <c r="Y19" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z19" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA19" s="9">
+        <v>1</v>
+      </c>
     </row>
-    <row r="20" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>2120</v>
       </c>
@@ -2269,9 +2516,20 @@
       <c r="W20" s="9">
         <v>0</v>
       </c>
-      <c r="X20" s="10"/>
+      <c r="X20" s="10">
+        <v>1</v>
+      </c>
+      <c r="Y20" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z20" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA20" s="9">
+        <v>1</v>
+      </c>
     </row>
-    <row r="21" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>2130</v>
       </c>
@@ -2348,9 +2606,20 @@
       <c r="W21" s="9">
         <v>0</v>
       </c>
-      <c r="X21" s="10"/>
+      <c r="X21" s="10">
+        <v>1</v>
+      </c>
+      <c r="Y21" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z21" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA21" s="9">
+        <v>1</v>
+      </c>
     </row>
-    <row r="22" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>2210</v>
       </c>
@@ -2427,9 +2696,20 @@
       <c r="W22" s="9">
         <v>0</v>
       </c>
-      <c r="X22" s="10"/>
+      <c r="X22" s="10">
+        <v>1</v>
+      </c>
+      <c r="Y22" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z22" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA22" s="9">
+        <v>1</v>
+      </c>
     </row>
-    <row r="23" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>2220</v>
       </c>
@@ -2506,9 +2786,20 @@
       <c r="W23" s="9">
         <v>0</v>
       </c>
-      <c r="X23" s="10"/>
+      <c r="X23" s="10">
+        <v>1</v>
+      </c>
+      <c r="Y23" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z23" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA23" s="9">
+        <v>1</v>
+      </c>
     </row>
-    <row r="24" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>2230</v>
       </c>
@@ -2585,9 +2876,20 @@
       <c r="W24" s="9">
         <v>0</v>
       </c>
-      <c r="X24" s="10"/>
+      <c r="X24" s="10">
+        <v>1</v>
+      </c>
+      <c r="Y24" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z24" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA24" s="9">
+        <v>1</v>
+      </c>
     </row>
-    <row r="25" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>2310</v>
       </c>
@@ -2664,9 +2966,20 @@
       <c r="W25" s="9">
         <v>0</v>
       </c>
-      <c r="X25" s="10"/>
+      <c r="X25" s="10">
+        <v>1</v>
+      </c>
+      <c r="Y25" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z25" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA25" s="9">
+        <v>1</v>
+      </c>
     </row>
-    <row r="26" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>2410</v>
       </c>
@@ -2743,9 +3056,20 @@
       <c r="W26" s="9">
         <v>0</v>
       </c>
-      <c r="X26" s="10"/>
+      <c r="X26" s="10">
+        <v>1</v>
+      </c>
+      <c r="Y26" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z26" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA26" s="9">
+        <v>1</v>
+      </c>
     </row>
-    <row r="27" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>2420</v>
       </c>
@@ -2822,9 +3146,20 @@
       <c r="W27" s="9">
         <v>0</v>
       </c>
-      <c r="X27" s="10"/>
+      <c r="X27" s="10">
+        <v>1</v>
+      </c>
+      <c r="Y27" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z27" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA27" s="9">
+        <v>1</v>
+      </c>
     </row>
-    <row r="28" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>2430</v>
       </c>
@@ -2901,9 +3236,20 @@
       <c r="W28" s="9">
         <v>0</v>
       </c>
-      <c r="X28" s="10"/>
+      <c r="X28" s="10">
+        <v>1</v>
+      </c>
+      <c r="Y28" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z28" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA28" s="9">
+        <v>1</v>
+      </c>
     </row>
-    <row r="29" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>2440</v>
       </c>
@@ -2980,9 +3326,20 @@
       <c r="W29" s="9">
         <v>0</v>
       </c>
-      <c r="X29" s="10"/>
+      <c r="X29" s="10">
+        <v>1</v>
+      </c>
+      <c r="Y29" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z29" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA29" s="9">
+        <v>1</v>
+      </c>
     </row>
-    <row r="30" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>3110</v>
       </c>
@@ -3003,48 +3360,48 @@
         <v>1311.85356095887</v>
       </c>
       <c r="G30" s="3">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="H30" s="3">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="I30" s="3">
         <v>1</v>
       </c>
       <c r="J30" s="3">
         <f t="shared" si="1"/>
-        <v>472.26728194519319</v>
+        <v>0</v>
       </c>
       <c r="K30" s="3">
         <v>0.5</v>
       </c>
       <c r="L30" s="3">
         <f t="shared" si="2"/>
-        <v>236.1336409725966</v>
+        <v>0</v>
       </c>
       <c r="M30" s="3">
-        <v>7.0000000000000007E-2</v>
+        <v>0</v>
       </c>
       <c r="N30" s="3">
         <f t="shared" si="3"/>
-        <v>33.058709736163529</v>
+        <v>0</v>
       </c>
       <c r="O30" s="3">
         <f t="shared" si="4"/>
-        <v>16.529354868081764</v>
+        <v>0</v>
       </c>
       <c r="P30" s="3">
         <v>0</v>
       </c>
       <c r="Q30" s="3">
         <f t="shared" si="5"/>
-        <v>49.58806460424529</v>
+        <v>0</v>
       </c>
       <c r="R30" s="9">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="S30" s="9">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="T30" s="9">
         <v>0</v>
@@ -3058,9 +3415,20 @@
       <c r="W30" s="9">
         <v>0</v>
       </c>
-      <c r="X30" s="10"/>
+      <c r="X30" s="10">
+        <v>0</v>
+      </c>
+      <c r="Y30" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z30" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA30" s="9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="31" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>3120</v>
       </c>
@@ -3081,48 +3449,48 @@
         <v>1311.85356095887</v>
       </c>
       <c r="G31" s="3">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="H31" s="3">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="I31" s="3">
         <v>1</v>
       </c>
       <c r="J31" s="3">
         <f t="shared" si="1"/>
-        <v>472.26728194519319</v>
+        <v>0</v>
       </c>
       <c r="K31" s="3">
         <v>0.5</v>
       </c>
       <c r="L31" s="3">
         <f t="shared" si="2"/>
-        <v>236.1336409725966</v>
+        <v>0</v>
       </c>
       <c r="M31" s="3">
-        <v>7.0000000000000007E-2</v>
+        <v>0</v>
       </c>
       <c r="N31" s="3">
         <f t="shared" si="3"/>
-        <v>33.058709736163529</v>
+        <v>0</v>
       </c>
       <c r="O31" s="3">
         <f t="shared" si="4"/>
-        <v>16.529354868081764</v>
+        <v>0</v>
       </c>
       <c r="P31" s="3">
         <v>0</v>
       </c>
       <c r="Q31" s="3">
         <f t="shared" si="5"/>
-        <v>49.58806460424529</v>
+        <v>0</v>
       </c>
       <c r="R31" s="9">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="S31" s="9">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="T31" s="9">
         <v>0</v>
@@ -3136,9 +3504,20 @@
       <c r="W31" s="9">
         <v>0</v>
       </c>
-      <c r="X31" s="10"/>
+      <c r="X31" s="10">
+        <v>0</v>
+      </c>
+      <c r="Y31" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z31" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA31" s="9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="32" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>3130</v>
       </c>
@@ -3159,48 +3538,48 @@
         <v>1311.85356095887</v>
       </c>
       <c r="G32" s="3">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="H32" s="3">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="I32" s="3">
         <v>1</v>
       </c>
       <c r="J32" s="3">
         <f t="shared" si="1"/>
-        <v>472.26728194519319</v>
+        <v>0</v>
       </c>
       <c r="K32" s="3">
         <v>0.5</v>
       </c>
       <c r="L32" s="3">
         <f t="shared" si="2"/>
-        <v>236.1336409725966</v>
+        <v>0</v>
       </c>
       <c r="M32" s="3">
-        <v>7.0000000000000007E-2</v>
+        <v>0</v>
       </c>
       <c r="N32" s="3">
         <f t="shared" si="3"/>
-        <v>33.058709736163529</v>
+        <v>0</v>
       </c>
       <c r="O32" s="3">
         <f t="shared" si="4"/>
-        <v>16.529354868081764</v>
+        <v>0</v>
       </c>
       <c r="P32" s="3">
         <v>0</v>
       </c>
       <c r="Q32" s="3">
         <f t="shared" si="5"/>
-        <v>49.58806460424529</v>
+        <v>0</v>
       </c>
       <c r="R32" s="9">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="S32" s="9">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="T32" s="9">
         <v>0</v>
@@ -3214,9 +3593,20 @@
       <c r="W32" s="9">
         <v>0</v>
       </c>
-      <c r="X32" s="10"/>
+      <c r="X32" s="10">
+        <v>0</v>
+      </c>
+      <c r="Y32" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z32" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA32" s="9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="33" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>3210</v>
       </c>
@@ -3292,9 +3682,20 @@
       <c r="W33" s="9">
         <v>0</v>
       </c>
-      <c r="X33" s="10"/>
+      <c r="X33" s="10">
+        <v>1</v>
+      </c>
+      <c r="Y33" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z33" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA33" s="9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="34" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>3220</v>
       </c>
@@ -3370,9 +3771,20 @@
       <c r="W34" s="9">
         <v>0</v>
       </c>
-      <c r="X34" s="10"/>
+      <c r="X34" s="10">
+        <v>1</v>
+      </c>
+      <c r="Y34" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z34" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA34" s="9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="35" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>3230</v>
       </c>
@@ -3448,9 +3860,20 @@
       <c r="W35" s="9">
         <v>0</v>
       </c>
-      <c r="X35" s="10"/>
+      <c r="X35" s="10">
+        <v>1</v>
+      </c>
+      <c r="Y35" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z35" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA35" s="9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="36" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>3240</v>
       </c>
@@ -3526,9 +3949,20 @@
       <c r="W36" s="9">
         <v>0</v>
       </c>
-      <c r="X36" s="10"/>
+      <c r="X36" s="10">
+        <v>1</v>
+      </c>
+      <c r="Y36" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z36" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA36" s="9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="37" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>3310</v>
       </c>
@@ -3604,9 +4038,20 @@
       <c r="W37" s="9">
         <v>0</v>
       </c>
-      <c r="X37" s="10"/>
+      <c r="X37" s="10">
+        <v>1</v>
+      </c>
+      <c r="Y37" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z37" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA37" s="9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="38" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>3320</v>
       </c>
@@ -3682,9 +4127,20 @@
       <c r="W38" s="9">
         <v>0</v>
       </c>
-      <c r="X38" s="10"/>
+      <c r="X38" s="10">
+        <v>1</v>
+      </c>
+      <c r="Y38" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z38" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA38" s="9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="39" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>3330</v>
       </c>
@@ -3760,9 +4216,20 @@
       <c r="W39" s="9">
         <v>0</v>
       </c>
-      <c r="X39" s="10"/>
+      <c r="X39" s="10">
+        <v>1</v>
+      </c>
+      <c r="Y39" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z39" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA39" s="9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="40" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>3340</v>
       </c>
@@ -3838,9 +4305,20 @@
       <c r="W40" s="9">
         <v>0</v>
       </c>
-      <c r="X40" s="10"/>
+      <c r="X40" s="10">
+        <v>1</v>
+      </c>
+      <c r="Y40" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z40" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA40" s="9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="41" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>3350</v>
       </c>
@@ -3916,9 +4394,20 @@
       <c r="W41" s="9">
         <v>0</v>
       </c>
-      <c r="X41" s="10"/>
+      <c r="X41" s="10">
+        <v>1</v>
+      </c>
+      <c r="Y41" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z41" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA41" s="9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="42" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>4000</v>
       </c>
@@ -3994,9 +4483,20 @@
       <c r="W42" s="9">
         <v>0</v>
       </c>
-      <c r="X42" s="10"/>
+      <c r="X42" s="10">
+        <v>1</v>
+      </c>
+      <c r="Y42" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z42" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA42" s="9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="43" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>5110</v>
       </c>
@@ -4072,9 +4572,20 @@
       <c r="W43" s="9">
         <v>0</v>
       </c>
-      <c r="X43" s="10"/>
+      <c r="X43" s="10">
+        <v>0</v>
+      </c>
+      <c r="Y43" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z43" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA43" s="9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="44" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>5120</v>
       </c>
@@ -4150,9 +4661,20 @@
       <c r="W44" s="9">
         <v>0</v>
       </c>
-      <c r="X44" s="10"/>
+      <c r="X44" s="10">
+        <v>0</v>
+      </c>
+      <c r="Y44" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z44" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA44" s="9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="45" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>5210</v>
       </c>
@@ -4228,9 +4750,20 @@
       <c r="W45" s="9">
         <v>0</v>
       </c>
-      <c r="X45" s="10"/>
+      <c r="X45" s="10">
+        <v>0</v>
+      </c>
+      <c r="Y45" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z45" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA45" s="9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="46" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>5220</v>
       </c>
@@ -4306,9 +4839,20 @@
       <c r="W46" s="9">
         <v>0</v>
       </c>
-      <c r="X46" s="10"/>
+      <c r="X46" s="10">
+        <v>0</v>
+      </c>
+      <c r="Y46" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z46" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA46" s="9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="47" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>5230</v>
       </c>
@@ -4384,7 +4928,18 @@
       <c r="W47" s="9">
         <v>0</v>
       </c>
-      <c r="X47" s="10"/>
+      <c r="X47" s="10">
+        <v>0</v>
+      </c>
+      <c r="Y47" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z47" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA47" s="9">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update for more readability
</commit_message>
<xml_diff>
--- a/LUISA_damage_info_curves.xlsx
+++ b/LUISA_damage_info_curves.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://deltares-my.sharepoint.com/personal/ted_buskop_deltares_nl/Documents/Documents/GitHub/FLOODS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="202" documentId="11_7BE859CF2764FA39C2903889AFA03F75A90CA07F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BEDE3814-E24C-4B07-9F9D-B3F09ECD9C36}"/>
+  <xr:revisionPtr revIDLastSave="203" documentId="11_7BE859CF2764FA39C2903889AFA03F75A90CA07F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7B2EFE48-8082-4C00-9EE8-C0502C6582C5}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -288,7 +288,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="#,##0.00%"/>
     <numFmt numFmtId="165" formatCode="#,##0%"/>
-    <numFmt numFmtId="167" formatCode="#,##0.000"/>
+    <numFmt numFmtId="166" formatCode="#,##0.000"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -450,19 +450,19 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="167" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
@@ -780,9 +780,9 @@
   </sheetPr>
   <dimension ref="A1:AI47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N45" sqref="N45"/>
+      <selection pane="bottomLeft" sqref="A1:AI6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>